<commit_message>
přidání testovacích scénářů, výkazu a zhodnocení práce
</commit_message>
<xml_diff>
--- a/K odevzdání/4. iterace/Testování/Testovací scénář - úprava jídelního lístku.xlsx
+++ b/K odevzdání/4. iterace/Testování/Testovací scénář - úprava jídelního lístku.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Název:</t>
   </si>
@@ -137,6 +138,21 @@
   </si>
   <si>
     <t>1.Zobrazení odpovídajících jídel</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>Zadání špatné ceny</t>
+  </si>
+  <si>
+    <t>Ověření, zda systém správně upozorní uživatele na problém s cenou u jídla</t>
+  </si>
+  <si>
+    <t>1.Zadám cenu, která nebude číslo (řetězec jiných znaků) u vybraného jídla</t>
+  </si>
+  <si>
+    <t>1.Systém mě upozorní na nepřevedení ceny jako řetězce na číslo</t>
   </si>
 </sst>
 </file>
@@ -756,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,4 +849,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>